<commit_message>
move mapping files, add PM ids that are part of ESPM meter data
</commit_message>
<xml_diff>
--- a/seed/tests/data/portfolio-manager-sample-with-crlf.xlsx
+++ b/seed/tests/data/portfolio-manager-sample-with-crlf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{676DFA5C-6DDE-9741-AFE1-5012B4F19A99}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC51B56-613D-734E-8004-42911BB7315E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17460" tabRatio="141" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -284,7 +284,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -627,7 +627,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D16"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -700,9 +700,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="65" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" ht="70" x14ac:dyDescent="0.15">
       <c r="A2">
-        <v>499045</v>
+        <v>5766973</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>596705</v>
+        <v>5766975</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -830,7 +830,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" ht="28" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>477198</v>
       </c>

</xml_diff>